<commit_message>
Empty, Full Profile fragment is designed.
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\20191119_android_python_carrental\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\CarRental-Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1054DC23-5163-4096-ACF3-74D9B2572FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F058F5E2-E3BB-4492-B0DF-70C5B0414686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{578811D6-0A5B-49C7-8281-BC532FB84A0E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>sign-up</t>
   </si>
@@ -94,6 +94,101 @@
   </si>
   <si>
     <t>https://github.com/habitio/habit-android-sdk-sample</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Sign Up new user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"name": "Tiny",
+"email": "tiny9611@outlook.com",
+"phone": "+8613522171058"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+success: true/false
+data {
+message:“invalid_email”
+}
+</t>
+  </si>
+  <si>
+    <t>-invalid_email
+-invalid_name
+-invalid_phone</t>
+  </si>
+  <si>
+    <t>"phone":"+8613522171058"</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>possible values</t>
+  </si>
+  <si>
+    <t>send OTP codes through SMS or email</t>
+  </si>
+  <si>
+    <t>-invalid_phone
+-not_exising_user</t>
+  </si>
+  <si>
+    <t>verify otp code</t>
+  </si>
+  <si>
+    <t>"phone":"+8613522171058"
+"otp": "4444"</t>
+  </si>
+  <si>
+    <t>-invalid_phone
+-invalid_otp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+success: true/false
+data {
+message:“invalid_otp”
+token:"123456"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"token":"123456
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+success: true/false
+data {
+message:"invalid_otp"
+profile: {
+}
+}
+</t>
+  </si>
+  <si>
+    <t>-----</t>
   </si>
 </sst>
 </file>
@@ -138,9 +233,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -456,89 +563,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC34131-F8D2-4DED-8113-B757DACE3ECA}">
-  <dimension ref="B4:C19"/>
+  <dimension ref="A3:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -547,7 +767,7 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -555,7 +775,7 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -565,5 +785,6 @@
     <hyperlink ref="C19" r:id="rId2" xr:uid="{CDD9923E-3640-4A27-89F9-E5E1A85FA18D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>